<commit_message>
Sediki di update oleh Samuel
</commit_message>
<xml_diff>
--- a/backendd/hasil_evaluasi_model.xlsx
+++ b/backendd/hasil_evaluasi_model.xlsx
@@ -462,10 +462,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -475,10 +475,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -542,10 +542,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="n">
         <v>100</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>100</v>
@@ -594,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,10 +626,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>69.56521739130434</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Brute Force</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>30.43478260869566</v>
       </c>
     </row>
   </sheetData>
@@ -643,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,13 +693,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
         <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Brute Force</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>71.42857142857143</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +780,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,13 +838,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>192.168.0.10</t>
+          <t>96.0.4664.110</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
+        <is>
+          <t>SQL Injection: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>192.168.0.10</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>SQL Injection: 1</t>
         </is>

</xml_diff>